<commit_message>
Updated data for Figure 12
</commit_message>
<xml_diff>
--- a/ewhr/data/datasets/dataset_12.xlsx
+++ b/ewhr/data/datasets/dataset_12.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>Country</t>
   </si>
@@ -22,21 +22,27 @@
     <t>male</t>
   </si>
   <si>
+    <t>male_note</t>
+  </si>
+  <si>
     <t>female</t>
   </si>
   <si>
+    <t>female_note</t>
+  </si>
+  <si>
     <t>gap</t>
   </si>
   <si>
     <t>Bosnia and Herzegovina</t>
   </si>
   <si>
+    <t>Serbia</t>
+  </si>
+  <si>
     <t>Ukraine</t>
   </si>
   <si>
-    <t>Serbia</t>
-  </si>
-  <si>
     <t>Belarus</t>
   </si>
   <si>
@@ -71,6 +77,15 @@
   </si>
   <si>
     <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> x </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> y </t>
   </si>
 </sst>
 </file>
@@ -428,13 +443,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,230 +462,326 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>1.3</v>
+      <c r="D2" t="s">
+        <v>21</v>
       </c>
       <c r="E2">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
+        <v>152</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>183</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>114</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>1.6</v>
-      </c>
-      <c r="D3">
-        <v>2.2</v>
-      </c>
-      <c r="E3">
-        <v>-0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>5.6</v>
-      </c>
-      <c r="D4">
-        <v>2.4</v>
-      </c>
-      <c r="E4">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>2.6</v>
-      </c>
-      <c r="D5">
-        <v>2.8</v>
-      </c>
-      <c r="E5">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>4.9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1">
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1">
+        <v>140</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>21.3</v>
-      </c>
-      <c r="D8">
-        <v>7.8</v>
-      </c>
-      <c r="E8">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>13.5</v>
-      </c>
-      <c r="D9">
-        <v>9.4</v>
-      </c>
-      <c r="E9">
-        <v>4.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>14.2</v>
-      </c>
-      <c r="D10">
-        <v>12.6</v>
-      </c>
-      <c r="E10">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
-        <v>11</v>
+        <v>173</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11">
-        <v>13.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C12">
-        <v>36.6</v>
-      </c>
-      <c r="D12">
-        <v>23.8</v>
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
       </c>
       <c r="E12">
-        <v>12.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>179</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13">
-        <v>29.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C14">
-        <v>63.1</v>
-      </c>
-      <c r="D14">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14">
         <v>39</v>
       </c>
-      <c r="E14">
-        <v>24.1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
-        <v>10</v>
+        <v>171</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15">
-        <v>46.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15">
+        <v>47</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>189</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C16">
-        <v>62.8</v>
-      </c>
-      <c r="D16">
         <v>63</v>
       </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
       <c r="E16">
-        <v>-0.200000000000003</v>
+        <v>63</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>